<commit_message>
Fixed issue 6993 - When changing a cell's data type from number to text it will no longer preserve the formatting (as it happens with Excel)
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
@@ -82,13 +82,13 @@
     <x:t>Date to Text:</x:t>
   </x:si>
   <x:si>
-    <x:t>09-02-10</x:t>
+    <x:t>40423</x:t>
   </x:si>
   <x:si>
     <x:t>DateTime to Text:</x:t>
   </x:si>
   <x:si>
-    <x:t>9/2/10 1:45</x:t>
+    <x:t>40423.5731712963</x:t>
   </x:si>
   <x:si>
     <x:t>Boolean to Text:</x:t>
@@ -100,6 +100,9 @@
     <x:t>TimeSpan to Text:</x:t>
   </x:si>
   <x:si>
+    <x:t>1.40650462962963</x:t>
+  </x:si>
+  <x:si>
     <x:t>Text to Date:</x:t>
   </x:si>
   <x:si>
@@ -121,13 +124,10 @@
     <x:t>Formatted Date to Text:</x:t>
   </x:si>
   <x:si>
-    <x:t>2010-09-02</x:t>
-  </x:si>
-  <x:si>
     <x:t>Formatted Number to Text:</x:t>
   </x:si>
   <x:si>
-    <x:t>12,345.68</x:t>
+    <x:t>12345.6789</x:t>
   </x:si>
   <x:si>
     <x:t>Blank Text:</x:t>
@@ -743,12 +743,12 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C24" s="10" t="s">
-        <x:v>19</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="B25" s="7" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C25" s="8">
         <x:v>40423</x:v>
@@ -756,7 +756,7 @@
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="B26" s="7" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C26" s="9">
         <x:v>40423.5731712963</x:v>
@@ -764,7 +764,7 @@
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="B27" s="7" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C27" s="7" t="b">
         <x:v>1</x:v>
@@ -772,7 +772,7 @@
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="B28" s="7" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C28" s="7" t="n">
         <x:v>123.45</x:v>
@@ -780,7 +780,7 @@
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="B29" s="7" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C29" s="11" t="n">
         <x:v>123.45</x:v>
@@ -788,7 +788,7 @@
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="B30" s="7" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C30" s="10" t="n">
         <x:v>1.40650462962963</x:v>
@@ -796,10 +796,10 @@
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="B32" s="7" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C32" s="12" t="s">
-        <x:v>35</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">

</xml_diff>

<commit_message>
Removed cell.GetRichText() as it's redundant to cell.RichText
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataTypes.xlsx
@@ -578,7 +578,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C37"/>
+  <x:dimension ref="A1:C38"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -825,6 +825,9 @@
           <x:t>Not Shared</x:t>
         </x:is>
       </x:c>
+    </x:row>
+    <x:row r="38" spans="1:3">
+      <x:c r="B38" s="7" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>